<commit_message>
Signed-off-by: IVAN KALENSKY <imitatehappiness@mail.ru>
</commit_message>
<xml_diff>
--- a/converter/data/item_data.xlsx
+++ b/converter/data/item_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imitatehappiness\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\imitatehappiness\devel\godot\GDAdvancedInventorySystem\converter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B72CB9-75AF-4AE3-B93D-AE87A782BD4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F9FFF9C-8F37-4A9D-92F0-F228D9006306}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1470" yWindow="1470" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4830" yWindow="3225" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -424,10 +424,14 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="5" max="5" width="16.42578125" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -510,10 +514,10 @@
       <c r="F3" s="3" t="b">
         <v>0</v>
       </c>
-      <c r="G3" s="2">
-        <v>60</v>
-      </c>
-      <c r="H3" s="1"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="1">
+        <v>10</v>
+      </c>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1"/>

</xml_diff>